<commit_message>
Commit Code by Deepak
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Navia Benefit\Navia\DocumentUnderstandingProcess3\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Navia Benefit\Navia-DU-Framework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7230"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7230" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="212">
   <si>
     <t>Name</t>
   </si>
@@ -652,6 +652,12 @@
   </si>
   <si>
     <t>Shared</t>
+  </si>
+  <si>
+    <t>DocumentFolderLocation</t>
+  </si>
+  <si>
+    <t>OutputFolder</t>
   </si>
 </sst>
 </file>
@@ -1052,7 +1058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z984"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -3693,8 +3699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA996"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3924,8 +3930,28 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:27" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:27" ht="14.25" customHeight="1">
+      <c r="A15" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B15" t="s">
+        <v>210</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>211</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>209</v>
+      </c>
+    </row>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>

</xml_diff>